<commit_message>
Fix dupe chairs on import
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/2021_sessions.xlsx
+++ b/app-server/src/main/resources/2021_sessions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/Downloads/cloudhubs/sac2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21074BF6-D149-8743-8A4E-CE7FEB1A8F71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7A0B61-6364-FA47-9AE9-4428C33EAFF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="19160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Session Chairs" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="638">
   <si>
     <t>Host</t>
   </si>
@@ -1491,9 +1491,6 @@
   </si>
   <si>
     <t>andrea.pedrotti@isti.cnr.it</t>
-  </si>
-  <si>
-    <t>1337 (SONAMA)</t>
   </si>
   <si>
     <t>Maurizio Leotta</t>
@@ -2429,29 +2426,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4271,7 +4268,7 @@
         <v>44278</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>114</v>
@@ -4321,7 +4318,7 @@
         <v>44278</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>114</v>
@@ -4365,13 +4362,13 @@
         <v>44278</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F48" s="10">
         <v>44278</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>119</v>
@@ -4409,13 +4406,13 @@
         <v>44278</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F49" s="10">
         <v>44278</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>119</v>
@@ -4453,13 +4450,13 @@
         <v>44278</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F50" s="10">
         <v>44278</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>30</v>
@@ -4503,13 +4500,13 @@
         <v>44278</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F51" s="10">
         <v>44279</v>
       </c>
       <c r="G51" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>30</v>
@@ -4553,13 +4550,13 @@
         <v>44278</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F52" s="10">
         <v>44278</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>30</v>
@@ -4603,13 +4600,13 @@
         <v>44279</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F53" s="10">
         <v>44279</v>
       </c>
       <c r="G53" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>30</v>
@@ -4689,7 +4686,7 @@
         <v>44278</v>
       </c>
       <c r="G55" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>123</v>
@@ -4739,7 +4736,7 @@
         <v>44278</v>
       </c>
       <c r="G56" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>123</v>
@@ -4783,13 +4780,13 @@
         <v>44278</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F57" s="10">
         <v>44278</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>127</v>
@@ -4841,13 +4838,13 @@
         <v>44278</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F58" s="10">
         <v>44278</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>127</v>
@@ -4899,13 +4896,13 @@
         <v>44278</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F59" s="10">
         <v>44278</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>135</v>
@@ -4959,13 +4956,13 @@
         <v>44278</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F60" s="10">
         <v>44279</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>135</v>
@@ -5019,13 +5016,13 @@
         <v>44278</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F61" s="10">
         <v>44278</v>
       </c>
       <c r="G61" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>144</v>
@@ -5072,13 +5069,13 @@
         <v>44279</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F62" s="10">
         <v>44279</v>
       </c>
       <c r="G62" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>144</v>
@@ -5162,7 +5159,7 @@
         <v>44278</v>
       </c>
       <c r="G64" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>30</v>
@@ -5212,7 +5209,7 @@
         <v>44278</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>30</v>
@@ -5256,13 +5253,13 @@
         <v>44278</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F66" s="10">
         <v>44278</v>
       </c>
       <c r="G66" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>30</v>
@@ -5306,13 +5303,13 @@
         <v>44278</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F67" s="10">
         <v>44278</v>
       </c>
       <c r="G67" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>30</v>
@@ -5356,13 +5353,13 @@
         <v>44278</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F68" s="10">
         <v>44278</v>
       </c>
       <c r="G68" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>154</v>
@@ -5414,13 +5411,13 @@
         <v>44278</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F69" s="10">
         <v>44279</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>154</v>
@@ -5472,13 +5469,13 @@
         <v>44278</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F70" s="10">
         <v>44278</v>
       </c>
       <c r="G70" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>160</v>
@@ -5530,13 +5527,13 @@
         <v>44279</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F71" s="10">
         <v>44279</v>
       </c>
       <c r="G71" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>160</v>
@@ -5624,7 +5621,7 @@
         <v>44278</v>
       </c>
       <c r="G73" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>167</v>
@@ -5674,7 +5671,7 @@
         <v>44278</v>
       </c>
       <c r="G74" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>167</v>
@@ -5718,13 +5715,13 @@
         <v>44278</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F75" s="10">
         <v>44278</v>
       </c>
       <c r="G75" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>169</v>
@@ -5768,13 +5765,13 @@
         <v>44278</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F76" s="10">
         <v>44278</v>
       </c>
       <c r="G76" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>169</v>
@@ -5818,13 +5815,13 @@
         <v>44278</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F77" s="10">
         <v>44278</v>
       </c>
       <c r="G77" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>172</v>
@@ -5876,13 +5873,13 @@
         <v>44278</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F78" s="10">
         <v>44279</v>
       </c>
       <c r="G78" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>172</v>
@@ -5934,13 +5931,13 @@
         <v>44278</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F79" s="10">
         <v>44278</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>179</v>
@@ -5988,13 +5985,13 @@
         <v>44279</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F80" s="10">
         <v>44279</v>
       </c>
       <c r="G80" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>179</v>
@@ -6078,7 +6075,7 @@
         <v>44278</v>
       </c>
       <c r="G82" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>184</v>
@@ -6132,7 +6129,7 @@
         <v>44278</v>
       </c>
       <c r="G83" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>184</v>
@@ -6178,13 +6175,13 @@
         <v>44278</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F84" s="10">
         <v>44278</v>
       </c>
       <c r="G84" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>188</v>
@@ -6236,13 +6233,13 @@
         <v>44278</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F85" s="10">
         <v>44278</v>
       </c>
       <c r="G85" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>188</v>
@@ -6294,13 +6291,13 @@
         <v>44278</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F86" s="10">
         <v>44278</v>
       </c>
       <c r="G86" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>192</v>
@@ -6352,13 +6349,13 @@
         <v>44278</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F87" s="10">
         <v>44279</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>192</v>
@@ -6410,13 +6407,13 @@
         <v>44278</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F88" s="10">
         <v>44278</v>
       </c>
       <c r="G88" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>192</v>
@@ -6454,13 +6451,13 @@
         <v>44279</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F89" s="10">
         <v>44279</v>
       </c>
       <c r="G89" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>192</v>
@@ -6620,7 +6617,7 @@
         <v>44279</v>
       </c>
       <c r="G94" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>135</v>
@@ -6680,7 +6677,7 @@
         <v>44279</v>
       </c>
       <c r="G95" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>135</v>
@@ -6732,13 +6729,13 @@
         <v>44279</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F96" s="10">
         <v>44279</v>
       </c>
       <c r="G96" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>213</v>
@@ -6788,13 +6785,13 @@
         <v>44279</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F97" s="10">
         <v>44279</v>
       </c>
       <c r="G97" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>213</v>
@@ -6844,13 +6841,13 @@
         <v>44279</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F98" s="10">
         <v>44279</v>
       </c>
       <c r="G98" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>218</v>
@@ -6894,13 +6891,13 @@
         <v>44279</v>
       </c>
       <c r="E99" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F99" s="10">
         <v>44280</v>
       </c>
       <c r="G99" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>218</v>
@@ -6944,13 +6941,13 @@
         <v>44279</v>
       </c>
       <c r="E100" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F100" s="10">
         <v>44279</v>
       </c>
       <c r="G100" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>221</v>
@@ -7002,13 +6999,13 @@
         <v>44280</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F101" s="10">
         <v>44280</v>
       </c>
       <c r="G101" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>221</v>
@@ -7096,7 +7093,7 @@
         <v>44279</v>
       </c>
       <c r="G103" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H103" s="29" t="s">
         <v>232</v>
@@ -7150,7 +7147,7 @@
         <v>44279</v>
       </c>
       <c r="G104" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H104" s="29" t="s">
         <v>232</v>
@@ -7198,13 +7195,13 @@
         <v>44279</v>
       </c>
       <c r="E105" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F105" s="10">
         <v>44279</v>
       </c>
       <c r="G105" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>237</v>
@@ -7248,13 +7245,13 @@
         <v>44279</v>
       </c>
       <c r="E106" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F106" s="10">
         <v>44279</v>
       </c>
       <c r="G106" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>237</v>
@@ -7298,13 +7295,13 @@
         <v>44279</v>
       </c>
       <c r="E107" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F107" s="10">
         <v>44279</v>
       </c>
       <c r="G107" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>240</v>
@@ -7348,13 +7345,13 @@
         <v>44279</v>
       </c>
       <c r="E108" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F108" s="10">
         <v>44280</v>
       </c>
       <c r="G108" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>240</v>
@@ -7398,13 +7395,13 @@
         <v>44279</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F109" s="10">
         <v>44279</v>
       </c>
       <c r="G109" s="31" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H109" s="2" t="s">
         <v>243</v>
@@ -7456,13 +7453,13 @@
         <v>44280</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F110" s="10">
         <v>44280</v>
       </c>
       <c r="G110" s="31" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H110" s="2" t="s">
         <v>243</v>
@@ -7550,7 +7547,7 @@
         <v>44279</v>
       </c>
       <c r="G112" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>251</v>
@@ -7600,7 +7597,7 @@
         <v>44279</v>
       </c>
       <c r="G113" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>251</v>
@@ -7644,13 +7641,13 @@
         <v>44279</v>
       </c>
       <c r="E114" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F114" s="10">
         <v>44279</v>
       </c>
       <c r="G114" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>255</v>
@@ -7694,13 +7691,13 @@
         <v>44279</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F115" s="10">
         <v>44279</v>
       </c>
       <c r="G115" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>255</v>
@@ -7744,13 +7741,13 @@
         <v>44279</v>
       </c>
       <c r="E116" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F116" s="10">
         <v>44279</v>
       </c>
       <c r="G116" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>257</v>
@@ -7794,13 +7791,13 @@
         <v>44279</v>
       </c>
       <c r="E117" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F117" s="10">
         <v>44280</v>
       </c>
       <c r="G117" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>257</v>
@@ -7844,13 +7841,13 @@
         <v>44279</v>
       </c>
       <c r="E118" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F118" s="10">
         <v>44279</v>
       </c>
       <c r="G118" s="31" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>258</v>
@@ -7900,13 +7897,13 @@
         <v>44280</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F119" s="10">
         <v>44280</v>
       </c>
       <c r="G119" s="31" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>258</v>
@@ -7992,7 +7989,7 @@
         <v>44279</v>
       </c>
       <c r="G121" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>81</v>
@@ -8042,7 +8039,7 @@
         <v>44279</v>
       </c>
       <c r="G122" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>81</v>
@@ -8086,13 +8083,13 @@
         <v>44279</v>
       </c>
       <c r="E123" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F123" s="10">
         <v>44279</v>
       </c>
       <c r="G123" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H123" s="2" t="s">
         <v>268</v>
@@ -8140,13 +8137,13 @@
         <v>44279</v>
       </c>
       <c r="E124" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F124" s="10">
         <v>44279</v>
       </c>
       <c r="G124" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>268</v>
@@ -8194,13 +8191,13 @@
         <v>44279</v>
       </c>
       <c r="E125" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F125" s="10">
         <v>44279</v>
       </c>
       <c r="G125" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>251</v>
@@ -8244,13 +8241,13 @@
         <v>44279</v>
       </c>
       <c r="E126" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F126" s="10">
         <v>44280</v>
       </c>
       <c r="G126" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>251</v>
@@ -8294,13 +8291,13 @@
         <v>44279</v>
       </c>
       <c r="E127" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F127" s="10">
         <v>44279</v>
       </c>
       <c r="G127" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>251</v>
@@ -8344,13 +8341,13 @@
         <v>44280</v>
       </c>
       <c r="E128" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F128" s="10">
         <v>44280</v>
       </c>
       <c r="G128" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>251</v>
@@ -8430,7 +8427,7 @@
         <v>44279</v>
       </c>
       <c r="G130" s="21" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>274</v>
@@ -8488,7 +8485,7 @@
         <v>44279</v>
       </c>
       <c r="G131" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>274</v>
@@ -8540,13 +8537,13 @@
         <v>44279</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F132" s="10">
         <v>44279</v>
       </c>
       <c r="G132" s="21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>279</v>
@@ -8590,13 +8587,13 @@
         <v>44279</v>
       </c>
       <c r="E133" s="21" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F133" s="10">
         <v>44279</v>
       </c>
       <c r="G133" s="21" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>279</v>
@@ -8640,13 +8637,13 @@
         <v>44279</v>
       </c>
       <c r="E134" s="21" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F134" s="10">
         <v>44279</v>
       </c>
       <c r="G134" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>283</v>
@@ -8694,13 +8691,13 @@
         <v>44279</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F135" s="10">
         <v>44280</v>
       </c>
       <c r="G135" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>283</v>
@@ -8748,13 +8745,13 @@
         <v>44279</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F136" s="10">
         <v>44279</v>
       </c>
       <c r="G136" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>283</v>
@@ -8802,13 +8799,13 @@
         <v>44280</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F137" s="10">
         <v>44280</v>
       </c>
       <c r="G137" s="21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H137" s="2" t="s">
         <v>283</v>
@@ -12746,10 +12743,10 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
+      <selection pane="bottomRight" activeCell="R96" sqref="R96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -12790,31 +12787,31 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="91" t="s">
         <v>372</v>
       </c>
       <c r="J1" s="81"/>
       <c r="K1" s="81"/>
       <c r="L1" s="81"/>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="91" t="s">
         <v>373</v>
       </c>
       <c r="N1" s="81"/>
       <c r="O1" s="81"/>
       <c r="P1" s="81"/>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="91" t="s">
         <v>374</v>
       </c>
       <c r="R1" s="81"/>
       <c r="S1" s="81"/>
       <c r="T1" s="81"/>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="91" t="s">
         <v>375</v>
       </c>
       <c r="V1" s="81"/>
       <c r="W1" s="81"/>
       <c r="X1" s="81"/>
-      <c r="Y1" s="84" t="s">
+      <c r="Y1" s="91" t="s">
         <v>376</v>
       </c>
       <c r="Z1" s="81"/>
@@ -12947,8 +12944,8 @@
       <c r="H4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="85" t="s">
-        <v>24</v>
+      <c r="I4" s="89">
+        <v>9991</v>
       </c>
       <c r="J4" s="49" t="s">
         <v>380</v>
@@ -13459,7 +13456,7 @@
       <c r="H21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="86">
+      <c r="I21" s="88">
         <v>1216</v>
       </c>
       <c r="J21" s="53" t="s">
@@ -13471,7 +13468,7 @@
       <c r="L21" s="54" t="s">
         <v>384</v>
       </c>
-      <c r="M21" s="86">
+      <c r="M21" s="88">
         <v>1218</v>
       </c>
       <c r="N21" s="53" t="s">
@@ -13483,7 +13480,7 @@
       <c r="P21" s="54" t="s">
         <v>387</v>
       </c>
-      <c r="Q21" s="86">
+      <c r="Q21" s="88">
         <v>1368</v>
       </c>
       <c r="R21" s="53" t="s">
@@ -13495,7 +13492,7 @@
       <c r="T21" s="54" t="s">
         <v>390</v>
       </c>
-      <c r="U21" s="86">
+      <c r="U21" s="88">
         <v>1433</v>
       </c>
       <c r="V21" s="53" t="s">
@@ -13601,7 +13598,7 @@
       <c r="H23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="86">
+      <c r="I23" s="88">
         <v>1147</v>
       </c>
       <c r="J23" s="53" t="s">
@@ -14356,9 +14353,9 @@
         <v>44278</v>
       </c>
       <c r="H46" s="52" t="s">
-        <v>623</v>
-      </c>
-      <c r="I46" s="86">
+        <v>622</v>
+      </c>
+      <c r="I46" s="88">
         <v>1691</v>
       </c>
       <c r="J46" s="55" t="s">
@@ -14370,7 +14367,7 @@
       <c r="L46" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="M46" s="86">
+      <c r="M46" s="88">
         <v>1017</v>
       </c>
       <c r="N46" s="56" t="s">
@@ -14380,7 +14377,7 @@
         <v>407</v>
       </c>
       <c r="P46" s="56"/>
-      <c r="Q46" s="86">
+      <c r="Q46" s="88">
         <v>1410</v>
       </c>
       <c r="R46" s="56" t="s">
@@ -14415,7 +14412,7 @@
         <v>44278</v>
       </c>
       <c r="H47" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I47" s="81"/>
       <c r="J47" s="55" t="s">
@@ -14462,13 +14459,13 @@
         <v>44278</v>
       </c>
       <c r="F48" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G48" s="50">
         <v>44278</v>
       </c>
       <c r="H48" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I48" s="83"/>
       <c r="M48" s="83"/>
@@ -14493,13 +14490,13 @@
         <v>44278</v>
       </c>
       <c r="F49" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G49" s="50">
         <v>44278</v>
       </c>
       <c r="H49" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I49" s="81"/>
       <c r="M49" s="81"/>
@@ -14524,13 +14521,13 @@
         <v>44278</v>
       </c>
       <c r="F50" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G50" s="50">
         <v>44278</v>
       </c>
       <c r="H50" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I50" s="83"/>
       <c r="M50" s="83"/>
@@ -14555,13 +14552,13 @@
         <v>44278</v>
       </c>
       <c r="F51" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G51" s="50">
         <v>44279</v>
       </c>
       <c r="H51" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I51" s="81"/>
       <c r="M51" s="81"/>
@@ -14586,13 +14583,13 @@
         <v>44278</v>
       </c>
       <c r="F52" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G52" s="50">
         <v>44278</v>
       </c>
       <c r="H52" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I52" s="83"/>
       <c r="M52" s="83"/>
@@ -14617,13 +14614,13 @@
         <v>44279</v>
       </c>
       <c r="F53" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G53" s="50">
         <v>44279</v>
       </c>
       <c r="H53" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I53" s="81"/>
       <c r="M53" s="81"/>
@@ -14678,11 +14675,11 @@
         <v>44278</v>
       </c>
       <c r="H55" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I55" s="83"/>
       <c r="M55" s="83"/>
-      <c r="Q55" s="90">
+      <c r="Q55" s="84">
         <v>1348</v>
       </c>
       <c r="R55" s="57" t="s">
@@ -14720,7 +14717,7 @@
         <v>44278</v>
       </c>
       <c r="H56" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I56" s="81"/>
       <c r="M56" s="81"/>
@@ -14754,13 +14751,13 @@
         <v>44278</v>
       </c>
       <c r="F57" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G57" s="50">
         <v>44278</v>
       </c>
       <c r="H57" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I57" s="87">
         <v>1647</v>
@@ -14807,13 +14804,13 @@
         <v>44278</v>
       </c>
       <c r="F58" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G58" s="50">
         <v>44278</v>
       </c>
       <c r="H58" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I58" s="81"/>
       <c r="J58" s="60" t="s">
@@ -14856,13 +14853,13 @@
         <v>44278</v>
       </c>
       <c r="F59" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G59" s="50">
         <v>44278</v>
       </c>
       <c r="H59" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I59" s="83"/>
       <c r="M59" s="83"/>
@@ -14887,13 +14884,13 @@
         <v>44278</v>
       </c>
       <c r="F60" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G60" s="50">
         <v>44279</v>
       </c>
       <c r="H60" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I60" s="81"/>
       <c r="M60" s="81"/>
@@ -14918,13 +14915,13 @@
         <v>44278</v>
       </c>
       <c r="F61" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G61" s="50">
         <v>44278</v>
       </c>
       <c r="H61" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I61" s="83">
         <v>1774</v>
@@ -14971,13 +14968,13 @@
         <v>44279</v>
       </c>
       <c r="F62" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G62" s="50">
         <v>44279</v>
       </c>
       <c r="H62" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I62" s="81"/>
       <c r="M62" s="51"/>
@@ -15032,7 +15029,7 @@
         <v>44278</v>
       </c>
       <c r="H64" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I64" s="83"/>
       <c r="M64" s="83"/>
@@ -15063,7 +15060,7 @@
         <v>44278</v>
       </c>
       <c r="H65" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I65" s="81"/>
       <c r="M65" s="81"/>
@@ -15088,13 +15085,13 @@
         <v>44278</v>
       </c>
       <c r="F66" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G66" s="50">
         <v>44278</v>
       </c>
       <c r="H66" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I66" s="83"/>
       <c r="M66" s="83"/>
@@ -15119,13 +15116,13 @@
         <v>44278</v>
       </c>
       <c r="F67" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G67" s="50">
         <v>44278</v>
       </c>
       <c r="H67" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I67" s="81"/>
       <c r="M67" s="81"/>
@@ -15150,13 +15147,13 @@
         <v>44278</v>
       </c>
       <c r="F68" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G68" s="50">
         <v>44278</v>
       </c>
       <c r="H68" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I68" s="83">
         <v>1176</v>
@@ -15225,13 +15222,13 @@
         <v>44278</v>
       </c>
       <c r="F69" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G69" s="50">
         <v>44279</v>
       </c>
       <c r="H69" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I69" s="81"/>
       <c r="M69" s="81"/>
@@ -15256,13 +15253,13 @@
         <v>44278</v>
       </c>
       <c r="F70" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G70" s="50">
         <v>44278</v>
       </c>
       <c r="H70" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I70" s="83">
         <v>1219</v>
@@ -15295,13 +15292,13 @@
         <v>44279</v>
       </c>
       <c r="F71" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G71" s="50">
         <v>44279</v>
       </c>
       <c r="H71" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I71" s="81"/>
       <c r="M71" s="81"/>
@@ -15356,7 +15353,7 @@
         <v>44278</v>
       </c>
       <c r="H73" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I73" s="83"/>
       <c r="M73" s="83"/>
@@ -15387,7 +15384,7 @@
         <v>44278</v>
       </c>
       <c r="H74" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I74" s="81"/>
       <c r="M74" s="81"/>
@@ -15412,13 +15409,13 @@
         <v>44278</v>
       </c>
       <c r="F75" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G75" s="50">
         <v>44278</v>
       </c>
       <c r="H75" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I75" s="83">
         <v>1133</v>
@@ -15450,13 +15447,13 @@
         <v>44278</v>
       </c>
       <c r="F76" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G76" s="50">
         <v>44278</v>
       </c>
       <c r="H76" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I76" s="81"/>
       <c r="J76" s="62"/>
@@ -15491,13 +15488,13 @@
         <v>44278</v>
       </c>
       <c r="F77" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G77" s="50">
         <v>44278</v>
       </c>
       <c r="H77" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I77" s="83">
         <v>1047</v>
@@ -15566,13 +15563,13 @@
         <v>44278</v>
       </c>
       <c r="F78" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G78" s="50">
         <v>44279</v>
       </c>
       <c r="H78" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I78" s="81"/>
       <c r="J78" s="13" t="s">
@@ -15633,13 +15630,13 @@
         <v>44278</v>
       </c>
       <c r="F79" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G79" s="50">
         <v>44278</v>
       </c>
       <c r="H79" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I79" s="83"/>
       <c r="M79" s="83"/>
@@ -15664,13 +15661,13 @@
         <v>44279</v>
       </c>
       <c r="F80" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G80" s="50">
         <v>44279</v>
       </c>
       <c r="H80" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I80" s="81"/>
       <c r="M80" s="81"/>
@@ -15725,7 +15722,7 @@
         <v>44278</v>
       </c>
       <c r="H82" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I82" s="83"/>
       <c r="M82" s="83"/>
@@ -15756,7 +15753,7 @@
         <v>44278</v>
       </c>
       <c r="H83" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I83" s="81"/>
       <c r="M83" s="81"/>
@@ -15781,13 +15778,13 @@
         <v>44278</v>
       </c>
       <c r="F84" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G84" s="50">
         <v>44278</v>
       </c>
       <c r="H84" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I84" s="83">
         <v>1127</v>
@@ -15813,14 +15810,14 @@
       <c r="P84" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="Q84" s="83" t="s">
+      <c r="Q84" s="83">
+        <v>1337</v>
+      </c>
+      <c r="R84" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="R84" s="13" t="s">
+      <c r="S84" s="13" t="s">
         <v>457</v>
-      </c>
-      <c r="S84" s="13" t="s">
-        <v>458</v>
       </c>
       <c r="T84" s="39" t="s">
         <v>330</v>
@@ -15845,13 +15842,13 @@
         <v>44278</v>
       </c>
       <c r="F85" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G85" s="50">
         <v>44278</v>
       </c>
       <c r="H85" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I85" s="81"/>
       <c r="J85" s="13" t="s">
@@ -15875,10 +15872,10 @@
       </c>
       <c r="Q85" s="81"/>
       <c r="R85" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="S85" s="13" t="s">
         <v>457</v>
-      </c>
-      <c r="S85" s="13" t="s">
-        <v>458</v>
       </c>
       <c r="T85" s="64" t="s">
         <v>330</v>
@@ -15903,22 +15900,22 @@
         <v>44278</v>
       </c>
       <c r="F86" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G86" s="50">
         <v>44278</v>
       </c>
       <c r="H86" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I86" s="87">
         <v>1563</v>
       </c>
       <c r="J86" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="K86" s="23" t="s">
         <v>459</v>
-      </c>
-      <c r="K86" s="23" t="s">
-        <v>460</v>
       </c>
       <c r="L86" s="28" t="s">
         <v>194</v>
@@ -15927,10 +15924,10 @@
         <v>1402</v>
       </c>
       <c r="N86" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="O86" s="23" t="s">
         <v>461</v>
-      </c>
-      <c r="O86" s="23" t="s">
-        <v>462</v>
       </c>
       <c r="P86" s="28" t="s">
         <v>196</v>
@@ -15939,13 +15936,13 @@
         <v>1263</v>
       </c>
       <c r="R86" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="S86" s="23" t="s">
         <v>463</v>
       </c>
-      <c r="S86" s="23" t="s">
+      <c r="T86" s="23" t="s">
         <v>464</v>
-      </c>
-      <c r="T86" s="23" t="s">
-        <v>465</v>
       </c>
       <c r="U86" s="83"/>
       <c r="Y86" s="83"/>
@@ -15967,43 +15964,43 @@
         <v>44278</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G87" s="50">
         <v>44279</v>
       </c>
       <c r="H87" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I87" s="81"/>
       <c r="J87" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="K87" s="23" t="s">
         <v>459</v>
-      </c>
-      <c r="K87" s="23" t="s">
-        <v>460</v>
       </c>
       <c r="L87" s="28" t="s">
         <v>194</v>
       </c>
       <c r="M87" s="81"/>
       <c r="N87" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="O87" s="23" t="s">
         <v>461</v>
-      </c>
-      <c r="O87" s="23" t="s">
-        <v>462</v>
       </c>
       <c r="P87" s="28" t="s">
         <v>196</v>
       </c>
       <c r="Q87" s="81"/>
       <c r="R87" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="S87" s="23" t="s">
         <v>463</v>
       </c>
-      <c r="S87" s="23" t="s">
+      <c r="T87" s="23" t="s">
         <v>464</v>
-      </c>
-      <c r="T87" s="23" t="s">
-        <v>465</v>
       </c>
       <c r="U87" s="81"/>
       <c r="Y87" s="81"/>
@@ -16025,22 +16022,22 @@
         <v>44278</v>
       </c>
       <c r="F88" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G88" s="50">
         <v>44278</v>
       </c>
       <c r="H88" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I88" s="87">
         <v>1591</v>
       </c>
       <c r="J88" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="K88" s="23" t="s">
         <v>466</v>
-      </c>
-      <c r="K88" s="23" t="s">
-        <v>467</v>
       </c>
       <c r="L88" s="28" t="s">
         <v>199</v>
@@ -16049,25 +16046,25 @@
         <v>1364</v>
       </c>
       <c r="N88" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="O88" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="O88" s="23" t="s">
+      <c r="P88" s="28" t="s">
         <v>469</v>
-      </c>
-      <c r="P88" s="28" t="s">
-        <v>470</v>
       </c>
       <c r="Q88" s="87">
         <v>1069</v>
       </c>
       <c r="R88" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="S88" s="23" t="s">
         <v>471</v>
       </c>
-      <c r="S88" s="23" t="s">
+      <c r="T88" s="28" t="s">
         <v>472</v>
-      </c>
-      <c r="T88" s="28" t="s">
-        <v>473</v>
       </c>
       <c r="U88" s="83"/>
       <c r="Y88" s="83"/>
@@ -16089,43 +16086,43 @@
         <v>44279</v>
       </c>
       <c r="F89" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G89" s="50">
         <v>44279</v>
       </c>
       <c r="H89" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I89" s="81"/>
       <c r="J89" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="K89" s="23" t="s">
         <v>466</v>
-      </c>
-      <c r="K89" s="23" t="s">
-        <v>467</v>
       </c>
       <c r="L89" s="28" t="s">
         <v>199</v>
       </c>
       <c r="M89" s="81"/>
       <c r="N89" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="O89" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="O89" s="23" t="s">
+      <c r="P89" s="28" t="s">
         <v>469</v>
-      </c>
-      <c r="P89" s="28" t="s">
-        <v>470</v>
       </c>
       <c r="Q89" s="81"/>
       <c r="R89" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="S89" s="23" t="s">
         <v>471</v>
       </c>
-      <c r="S89" s="23" t="s">
+      <c r="T89" s="28" t="s">
         <v>472</v>
-      </c>
-      <c r="T89" s="28" t="s">
-        <v>473</v>
       </c>
       <c r="U89" s="81"/>
       <c r="Y89" s="81"/>
@@ -16254,7 +16251,7 @@
         <v>44279</v>
       </c>
       <c r="H94" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I94" s="83"/>
       <c r="M94" s="83"/>
@@ -16285,7 +16282,7 @@
         <v>44279</v>
       </c>
       <c r="H95" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I95" s="81"/>
       <c r="M95" s="81"/>
@@ -16310,13 +16307,13 @@
         <v>44279</v>
       </c>
       <c r="F96" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G96" s="50">
         <v>44279</v>
       </c>
       <c r="H96" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I96" s="83"/>
       <c r="M96" s="83"/>
@@ -16341,13 +16338,13 @@
         <v>44279</v>
       </c>
       <c r="F97" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G97" s="50">
         <v>44279</v>
       </c>
       <c r="H97" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I97" s="81"/>
       <c r="M97" s="81"/>
@@ -16372,61 +16369,61 @@
         <v>44279</v>
       </c>
       <c r="F98" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G98" s="50">
         <v>44279</v>
       </c>
       <c r="H98" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I98" s="83">
         <v>1541</v>
       </c>
       <c r="J98" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="K98" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="K98" s="11" t="s">
+      <c r="L98" s="11" t="s">
         <v>475</v>
-      </c>
-      <c r="L98" s="11" t="s">
-        <v>476</v>
       </c>
       <c r="M98" s="83">
         <v>1092</v>
       </c>
       <c r="N98" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="O98" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="O98" s="11" t="s">
+      <c r="P98" s="11" t="s">
         <v>478</v>
-      </c>
-      <c r="P98" s="11" t="s">
-        <v>479</v>
       </c>
       <c r="Q98" s="83">
         <v>1375</v>
       </c>
       <c r="R98" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="S98" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="S98" s="11" t="s">
+      <c r="T98" s="11" t="s">
         <v>481</v>
-      </c>
-      <c r="T98" s="11" t="s">
-        <v>482</v>
       </c>
       <c r="U98" s="83">
         <v>1558</v>
       </c>
       <c r="V98" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="W98" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="W98" s="11" t="s">
+      <c r="X98" s="11" t="s">
         <v>484</v>
-      </c>
-      <c r="X98" s="11" t="s">
-        <v>485</v>
       </c>
       <c r="Y98" s="83"/>
     </row>
@@ -16447,53 +16444,53 @@
         <v>44279</v>
       </c>
       <c r="F99" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G99" s="50">
         <v>44280</v>
       </c>
       <c r="H99" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I99" s="81"/>
       <c r="J99" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="K99" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="K99" s="11" t="s">
+      <c r="L99" s="11" t="s">
         <v>475</v>
-      </c>
-      <c r="L99" s="11" t="s">
-        <v>476</v>
       </c>
       <c r="M99" s="81"/>
       <c r="N99" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="O99" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="O99" s="11" t="s">
+      <c r="P99" s="11" t="s">
         <v>478</v>
-      </c>
-      <c r="P99" s="11" t="s">
-        <v>479</v>
       </c>
       <c r="Q99" s="81"/>
       <c r="R99" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="S99" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="S99" s="11" t="s">
+      <c r="T99" s="11" t="s">
         <v>481</v>
-      </c>
-      <c r="T99" s="11" t="s">
-        <v>482</v>
       </c>
       <c r="U99" s="81"/>
       <c r="V99" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="W99" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="W99" s="11" t="s">
+      <c r="X99" s="11" t="s">
         <v>484</v>
-      </c>
-      <c r="X99" s="11" t="s">
-        <v>485</v>
       </c>
       <c r="Y99" s="81"/>
     </row>
@@ -16514,61 +16511,61 @@
         <v>44279</v>
       </c>
       <c r="F100" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G100" s="50">
         <v>44279</v>
       </c>
       <c r="H100" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I100" s="83">
         <v>1326</v>
       </c>
       <c r="J100" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="K100" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="K100" s="11" t="s">
+      <c r="L100" s="11" t="s">
         <v>487</v>
-      </c>
-      <c r="L100" s="11" t="s">
-        <v>488</v>
       </c>
       <c r="M100" s="83">
         <v>1636</v>
       </c>
       <c r="N100" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="O100" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="O100" s="11" t="s">
+      <c r="P100" s="11" t="s">
         <v>490</v>
-      </c>
-      <c r="P100" s="11" t="s">
-        <v>491</v>
       </c>
       <c r="Q100" s="83">
         <v>1483</v>
       </c>
       <c r="R100" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="S100" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="S100" s="11" t="s">
+      <c r="T100" s="11" t="s">
         <v>493</v>
-      </c>
-      <c r="T100" s="11" t="s">
-        <v>494</v>
       </c>
       <c r="U100" s="83">
         <v>1682</v>
       </c>
       <c r="V100" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="W100" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="W100" s="11" t="s">
+      <c r="X100" s="11" t="s">
         <v>496</v>
-      </c>
-      <c r="X100" s="11" t="s">
-        <v>497</v>
       </c>
       <c r="Y100" s="83"/>
     </row>
@@ -16589,53 +16586,53 @@
         <v>44280</v>
       </c>
       <c r="F101" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G101" s="50">
         <v>44280</v>
       </c>
       <c r="H101" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I101" s="81"/>
       <c r="J101" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="K101" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="K101" s="11" t="s">
+      <c r="L101" s="11" t="s">
         <v>487</v>
-      </c>
-      <c r="L101" s="11" t="s">
-        <v>488</v>
       </c>
       <c r="M101" s="81"/>
       <c r="N101" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O101" s="11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="P101" s="11" t="s">
         <v>230</v>
       </c>
       <c r="Q101" s="81"/>
       <c r="R101" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="S101" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="S101" s="11" t="s">
+      <c r="T101" s="11" t="s">
         <v>493</v>
-      </c>
-      <c r="T101" s="11" t="s">
-        <v>494</v>
       </c>
       <c r="U101" s="81"/>
       <c r="V101" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="W101" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="W101" s="11" t="s">
+      <c r="X101" s="11" t="s">
         <v>496</v>
-      </c>
-      <c r="X101" s="11" t="s">
-        <v>497</v>
       </c>
       <c r="Y101" s="81"/>
     </row>
@@ -16686,16 +16683,16 @@
         <v>44279</v>
       </c>
       <c r="H103" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I103" s="83">
         <v>1781</v>
       </c>
       <c r="J103" s="25" t="s">
+        <v>498</v>
+      </c>
+      <c r="K103" s="13" t="s">
         <v>499</v>
-      </c>
-      <c r="K103" s="13" t="s">
-        <v>500</v>
       </c>
       <c r="L103" s="13" t="s">
         <v>431</v>
@@ -16728,17 +16725,17 @@
         <v>44279</v>
       </c>
       <c r="H104" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I104" s="81"/>
       <c r="J104" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="K104" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="L104" s="13" t="s">
         <v>501</v>
-      </c>
-      <c r="K104" s="13" t="s">
-        <v>500</v>
-      </c>
-      <c r="L104" s="13" t="s">
-        <v>502</v>
       </c>
       <c r="M104" s="81"/>
       <c r="Q104" s="81"/>
@@ -16762,37 +16759,37 @@
         <v>44279</v>
       </c>
       <c r="F105" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G105" s="50">
         <v>44279</v>
       </c>
       <c r="H105" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I105" s="83">
         <v>1793</v>
       </c>
       <c r="J105" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="K105" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="K105" s="13" t="s">
+      <c r="L105" s="13" t="s">
         <v>504</v>
-      </c>
-      <c r="L105" s="13" t="s">
-        <v>505</v>
       </c>
       <c r="M105" s="83">
         <v>1057</v>
       </c>
       <c r="N105" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="O105" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="O105" s="13" t="s">
+      <c r="P105" s="13" t="s">
         <v>507</v>
-      </c>
-      <c r="P105" s="13" t="s">
-        <v>508</v>
       </c>
       <c r="Q105" s="83"/>
       <c r="U105" s="83"/>
@@ -16815,33 +16812,33 @@
         <v>44279</v>
       </c>
       <c r="F106" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G106" s="50">
         <v>44279</v>
       </c>
       <c r="H106" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I106" s="81"/>
       <c r="J106" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="K106" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="K106" s="13" t="s">
+      <c r="L106" s="13" t="s">
         <v>504</v>
-      </c>
-      <c r="L106" s="13" t="s">
-        <v>505</v>
       </c>
       <c r="M106" s="81"/>
       <c r="N106" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="O106" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="O106" s="13" t="s">
+      <c r="P106" s="13" t="s">
         <v>507</v>
-      </c>
-      <c r="P106" s="13" t="s">
-        <v>508</v>
       </c>
       <c r="Q106" s="81"/>
       <c r="U106" s="81"/>
@@ -16864,13 +16861,13 @@
         <v>44279</v>
       </c>
       <c r="F107" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G107" s="50">
         <v>44279</v>
       </c>
       <c r="H107" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I107" s="83">
         <v>1482</v>
@@ -16903,13 +16900,13 @@
         <v>44279</v>
       </c>
       <c r="F108" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G108" s="50">
         <v>44280</v>
       </c>
       <c r="H108" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I108" s="81"/>
       <c r="M108" s="81"/>
@@ -16934,13 +16931,13 @@
         <v>44279</v>
       </c>
       <c r="F109" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G109" s="50">
         <v>44279</v>
       </c>
       <c r="H109" s="65" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I109" s="83"/>
       <c r="M109" s="83"/>
@@ -16965,13 +16962,13 @@
         <v>44280</v>
       </c>
       <c r="F110" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G110" s="50">
         <v>44280</v>
       </c>
       <c r="H110" s="65" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I110" s="81"/>
       <c r="M110" s="81"/>
@@ -17026,43 +17023,43 @@
         <v>44279</v>
       </c>
       <c r="H112" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I112" s="83">
         <v>1043</v>
       </c>
       <c r="J112" s="63" t="s">
+        <v>508</v>
+      </c>
+      <c r="K112" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="K112" s="13" t="s">
+      <c r="L112" s="63" t="s">
         <v>510</v>
-      </c>
-      <c r="L112" s="63" t="s">
-        <v>511</v>
       </c>
       <c r="M112" s="83">
         <v>1128</v>
       </c>
       <c r="N112" s="63" t="s">
+        <v>511</v>
+      </c>
+      <c r="O112" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="O112" s="13" t="s">
+      <c r="P112" s="63" t="s">
         <v>513</v>
-      </c>
-      <c r="P112" s="63" t="s">
-        <v>514</v>
       </c>
       <c r="Q112" s="83">
         <v>1231</v>
       </c>
       <c r="R112" s="63" t="s">
+        <v>514</v>
+      </c>
+      <c r="S112" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="S112" s="13" t="s">
+      <c r="T112" s="63" t="s">
         <v>516</v>
-      </c>
-      <c r="T112" s="63" t="s">
-        <v>517</v>
       </c>
       <c r="U112" s="83"/>
       <c r="Y112" s="83"/>
@@ -17090,37 +17087,37 @@
         <v>44279</v>
       </c>
       <c r="H113" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I113" s="81"/>
       <c r="J113" s="63" t="s">
+        <v>508</v>
+      </c>
+      <c r="K113" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="K113" s="13" t="s">
+      <c r="L113" s="63" t="s">
         <v>510</v>
-      </c>
-      <c r="L113" s="63" t="s">
-        <v>511</v>
       </c>
       <c r="M113" s="81"/>
       <c r="N113" s="63" t="s">
+        <v>511</v>
+      </c>
+      <c r="O113" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="O113" s="13" t="s">
+      <c r="P113" s="63" t="s">
         <v>513</v>
-      </c>
-      <c r="P113" s="63" t="s">
-        <v>514</v>
       </c>
       <c r="Q113" s="81"/>
       <c r="R113" s="63" t="s">
+        <v>514</v>
+      </c>
+      <c r="S113" s="13" t="s">
         <v>515</v>
       </c>
-      <c r="S113" s="13" t="s">
+      <c r="T113" s="63" t="s">
         <v>516</v>
-      </c>
-      <c r="T113" s="63" t="s">
-        <v>517</v>
       </c>
       <c r="U113" s="81"/>
       <c r="Y113" s="81"/>
@@ -17142,37 +17139,37 @@
         <v>44279</v>
       </c>
       <c r="F114" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G114" s="50">
         <v>44279</v>
       </c>
       <c r="H114" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I114" s="83">
         <v>1431</v>
       </c>
       <c r="J114" s="63" t="s">
+        <v>517</v>
+      </c>
+      <c r="K114" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="K114" s="13" t="s">
+      <c r="L114" s="63" t="s">
         <v>519</v>
-      </c>
-      <c r="L114" s="63" t="s">
-        <v>520</v>
       </c>
       <c r="M114" s="83">
         <v>1446</v>
       </c>
       <c r="N114" s="63" t="s">
+        <v>520</v>
+      </c>
+      <c r="O114" s="13" t="s">
         <v>521</v>
       </c>
-      <c r="O114" s="13" t="s">
+      <c r="P114" s="63" t="s">
         <v>522</v>
-      </c>
-      <c r="P114" s="63" t="s">
-        <v>523</v>
       </c>
       <c r="Q114" s="83"/>
       <c r="U114" s="83"/>
@@ -17195,33 +17192,33 @@
         <v>44279</v>
       </c>
       <c r="F115" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G115" s="50">
         <v>44279</v>
       </c>
       <c r="H115" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I115" s="81"/>
       <c r="J115" s="63" t="s">
+        <v>517</v>
+      </c>
+      <c r="K115" s="13" t="s">
         <v>518</v>
       </c>
-      <c r="K115" s="13" t="s">
+      <c r="L115" s="63" t="s">
         <v>519</v>
-      </c>
-      <c r="L115" s="63" t="s">
-        <v>520</v>
       </c>
       <c r="M115" s="81"/>
       <c r="N115" s="63" t="s">
+        <v>520</v>
+      </c>
+      <c r="O115" s="13" t="s">
         <v>521</v>
       </c>
-      <c r="O115" s="13" t="s">
+      <c r="P115" s="63" t="s">
         <v>522</v>
-      </c>
-      <c r="P115" s="63" t="s">
-        <v>523</v>
       </c>
       <c r="Q115" s="81"/>
       <c r="U115" s="81"/>
@@ -17244,61 +17241,61 @@
         <v>44279</v>
       </c>
       <c r="F116" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G116" s="50">
         <v>44279</v>
       </c>
       <c r="H116" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I116" s="83">
         <v>1659</v>
       </c>
       <c r="J116" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="K116" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="K116" s="13" t="s">
+      <c r="L116" s="13" t="s">
         <v>525</v>
-      </c>
-      <c r="L116" s="13" t="s">
-        <v>526</v>
       </c>
       <c r="M116" s="83">
         <v>1619</v>
       </c>
       <c r="N116" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="O116" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="O116" s="13" t="s">
+      <c r="P116" s="13" t="s">
         <v>528</v>
-      </c>
-      <c r="P116" s="13" t="s">
-        <v>529</v>
       </c>
       <c r="Q116" s="83">
         <v>1261</v>
       </c>
       <c r="R116" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="S116" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="T116" s="13" t="s">
         <v>530</v>
-      </c>
-      <c r="S116" s="13" t="s">
-        <v>507</v>
-      </c>
-      <c r="T116" s="13" t="s">
-        <v>531</v>
       </c>
       <c r="U116" s="83">
         <v>1543</v>
       </c>
       <c r="V116" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="W116" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="W116" s="13" t="s">
+      <c r="X116" s="66" t="s">
         <v>533</v>
-      </c>
-      <c r="X116" s="66" t="s">
-        <v>534</v>
       </c>
       <c r="Y116" s="83"/>
     </row>
@@ -17319,53 +17316,53 @@
         <v>44279</v>
       </c>
       <c r="F117" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G117" s="50">
         <v>44280</v>
       </c>
       <c r="H117" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I117" s="81"/>
       <c r="J117" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="K117" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="K117" s="13" t="s">
+      <c r="L117" s="13" t="s">
         <v>525</v>
-      </c>
-      <c r="L117" s="13" t="s">
-        <v>526</v>
       </c>
       <c r="M117" s="81"/>
       <c r="N117" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="O117" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="O117" s="13" t="s">
+      <c r="P117" s="13" t="s">
         <v>528</v>
-      </c>
-      <c r="P117" s="13" t="s">
-        <v>529</v>
       </c>
       <c r="Q117" s="81"/>
       <c r="R117" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="S117" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="T117" s="13" t="s">
         <v>530</v>
-      </c>
-      <c r="S117" s="13" t="s">
-        <v>507</v>
-      </c>
-      <c r="T117" s="13" t="s">
-        <v>531</v>
       </c>
       <c r="U117" s="81"/>
       <c r="V117" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="W117" s="66" t="s">
         <v>532</v>
       </c>
-      <c r="W117" s="66" t="s">
+      <c r="X117" s="66" t="s">
         <v>533</v>
-      </c>
-      <c r="X117" s="66" t="s">
-        <v>534</v>
       </c>
       <c r="Y117" s="81"/>
     </row>
@@ -17386,37 +17383,37 @@
         <v>44279</v>
       </c>
       <c r="F118" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G118" s="50">
         <v>44279</v>
       </c>
       <c r="H118" s="65" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I118" s="83">
         <v>1297</v>
       </c>
       <c r="J118" s="13" t="s">
+        <v>534</v>
+      </c>
+      <c r="K118" s="13" t="s">
+        <v>527</v>
+      </c>
+      <c r="L118" s="13" t="s">
         <v>535</v>
-      </c>
-      <c r="K118" s="13" t="s">
-        <v>528</v>
-      </c>
-      <c r="L118" s="13" t="s">
-        <v>536</v>
       </c>
       <c r="M118" s="83">
         <v>1757</v>
       </c>
       <c r="N118" s="13" t="s">
+        <v>536</v>
+      </c>
+      <c r="O118" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="O118" s="13" t="s">
+      <c r="P118" s="13" t="s">
         <v>538</v>
-      </c>
-      <c r="P118" s="13" t="s">
-        <v>539</v>
       </c>
       <c r="Q118" s="83"/>
       <c r="U118" s="83"/>
@@ -17439,33 +17436,33 @@
         <v>44280</v>
       </c>
       <c r="F119" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G119" s="50">
         <v>44280</v>
       </c>
       <c r="H119" s="65" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I119" s="81"/>
       <c r="J119" s="13" t="s">
+        <v>534</v>
+      </c>
+      <c r="K119" s="13" t="s">
+        <v>527</v>
+      </c>
+      <c r="L119" s="13" t="s">
         <v>535</v>
-      </c>
-      <c r="K119" s="13" t="s">
-        <v>528</v>
-      </c>
-      <c r="L119" s="13" t="s">
-        <v>536</v>
       </c>
       <c r="M119" s="81"/>
       <c r="N119" s="13" t="s">
+        <v>536</v>
+      </c>
+      <c r="O119" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="O119" s="13" t="s">
+      <c r="P119" s="13" t="s">
         <v>538</v>
-      </c>
-      <c r="P119" s="13" t="s">
-        <v>539</v>
       </c>
       <c r="Q119" s="81"/>
       <c r="U119" s="81"/>
@@ -17518,7 +17515,7 @@
         <v>44279</v>
       </c>
       <c r="H121" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I121" s="83">
         <v>1134</v>
@@ -17555,7 +17552,7 @@
         <v>44279</v>
       </c>
       <c r="H122" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I122" s="81"/>
       <c r="M122" s="81"/>
@@ -17580,13 +17577,13 @@
         <v>44279</v>
       </c>
       <c r="F123" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G123" s="50">
         <v>44279</v>
       </c>
       <c r="H123" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I123" s="83"/>
       <c r="M123" s="83"/>
@@ -17611,13 +17608,13 @@
         <v>44279</v>
       </c>
       <c r="F124" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G124" s="50">
         <v>44279</v>
       </c>
       <c r="H124" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I124" s="81"/>
       <c r="M124" s="81"/>
@@ -17642,61 +17639,61 @@
         <v>44279</v>
       </c>
       <c r="F125" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G125" s="50">
         <v>44279</v>
       </c>
       <c r="H125" s="52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I125" s="83">
         <v>1014</v>
       </c>
       <c r="J125" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="K125" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="K125" s="13" t="s">
+      <c r="L125" s="63" t="s">
         <v>541</v>
-      </c>
-      <c r="L125" s="63" t="s">
-        <v>542</v>
       </c>
       <c r="M125" s="83">
         <v>1039</v>
       </c>
       <c r="N125" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="O125" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="O125" s="13" t="s">
+      <c r="P125" s="63" t="s">
         <v>544</v>
-      </c>
-      <c r="P125" s="63" t="s">
-        <v>545</v>
       </c>
       <c r="Q125" s="83">
         <v>1061</v>
       </c>
       <c r="R125" s="13" t="s">
+        <v>545</v>
+      </c>
+      <c r="S125" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="T125" s="63" t="s">
         <v>546</v>
-      </c>
-      <c r="S125" s="13" t="s">
-        <v>513</v>
-      </c>
-      <c r="T125" s="63" t="s">
-        <v>547</v>
       </c>
       <c r="U125" s="83">
         <v>1106</v>
       </c>
       <c r="V125" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="W125" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="W125" s="13" t="s">
+      <c r="X125" s="63" t="s">
         <v>549</v>
-      </c>
-      <c r="X125" s="63" t="s">
-        <v>550</v>
       </c>
       <c r="Y125" s="83"/>
     </row>
@@ -17717,53 +17714,53 @@
         <v>44279</v>
       </c>
       <c r="F126" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G126" s="50">
         <v>44280</v>
       </c>
       <c r="H126" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I126" s="81"/>
       <c r="J126" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="K126" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="K126" s="13" t="s">
+      <c r="L126" s="63" t="s">
         <v>541</v>
-      </c>
-      <c r="L126" s="63" t="s">
-        <v>542</v>
       </c>
       <c r="M126" s="81"/>
       <c r="N126" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="O126" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="O126" s="13" t="s">
+      <c r="P126" s="63" t="s">
         <v>544</v>
-      </c>
-      <c r="P126" s="63" t="s">
-        <v>545</v>
       </c>
       <c r="Q126" s="81"/>
       <c r="R126" s="13" t="s">
+        <v>545</v>
+      </c>
+      <c r="S126" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="T126" s="63" t="s">
         <v>546</v>
-      </c>
-      <c r="S126" s="13" t="s">
-        <v>513</v>
-      </c>
-      <c r="T126" s="63" t="s">
-        <v>547</v>
       </c>
       <c r="U126" s="81"/>
       <c r="V126" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="W126" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="W126" s="13" t="s">
+      <c r="X126" s="63" t="s">
         <v>549</v>
-      </c>
-      <c r="X126" s="63" t="s">
-        <v>550</v>
       </c>
       <c r="Y126" s="81"/>
     </row>
@@ -17784,61 +17781,61 @@
         <v>44279</v>
       </c>
       <c r="F127" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G127" s="50">
         <v>44279</v>
       </c>
       <c r="H127" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I127" s="83">
         <v>1291</v>
       </c>
       <c r="J127" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="K127" s="13" t="s">
         <v>551</v>
       </c>
-      <c r="K127" s="13" t="s">
+      <c r="L127" s="63" t="s">
         <v>552</v>
-      </c>
-      <c r="L127" s="63" t="s">
-        <v>553</v>
       </c>
       <c r="M127" s="83">
         <v>1313</v>
       </c>
       <c r="N127" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="O127" s="13" t="s">
         <v>554</v>
       </c>
-      <c r="O127" s="13" t="s">
+      <c r="P127" s="63" t="s">
         <v>555</v>
-      </c>
-      <c r="P127" s="63" t="s">
-        <v>556</v>
       </c>
       <c r="Q127" s="83">
         <v>1322</v>
       </c>
       <c r="R127" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="S127" s="13" t="s">
         <v>557</v>
       </c>
-      <c r="S127" s="13" t="s">
+      <c r="T127" s="63" t="s">
         <v>558</v>
-      </c>
-      <c r="T127" s="63" t="s">
-        <v>559</v>
       </c>
       <c r="U127" s="83">
         <v>1463</v>
       </c>
       <c r="V127" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="W127" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="W127" s="13" t="s">
+      <c r="X127" s="63" t="s">
         <v>561</v>
-      </c>
-      <c r="X127" s="63" t="s">
-        <v>562</v>
       </c>
       <c r="Y127" s="83"/>
     </row>
@@ -17859,53 +17856,53 @@
         <v>44280</v>
       </c>
       <c r="F128" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G128" s="50">
         <v>44280</v>
       </c>
       <c r="H128" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I128" s="81"/>
       <c r="J128" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="K128" s="13" t="s">
         <v>551</v>
       </c>
-      <c r="K128" s="13" t="s">
+      <c r="L128" s="63" t="s">
         <v>552</v>
-      </c>
-      <c r="L128" s="63" t="s">
-        <v>553</v>
       </c>
       <c r="M128" s="81"/>
       <c r="N128" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="O128" s="13" t="s">
         <v>554</v>
       </c>
-      <c r="O128" s="13" t="s">
+      <c r="P128" s="63" t="s">
         <v>555</v>
-      </c>
-      <c r="P128" s="63" t="s">
-        <v>556</v>
       </c>
       <c r="Q128" s="81"/>
       <c r="R128" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="S128" s="13" t="s">
         <v>557</v>
       </c>
-      <c r="S128" s="13" t="s">
+      <c r="T128" s="63" t="s">
         <v>558</v>
-      </c>
-      <c r="T128" s="63" t="s">
-        <v>559</v>
       </c>
       <c r="U128" s="81"/>
       <c r="V128" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="W128" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="W128" s="13" t="s">
+      <c r="X128" s="63" t="s">
         <v>561</v>
-      </c>
-      <c r="X128" s="63" t="s">
-        <v>562</v>
       </c>
       <c r="Y128" s="81"/>
     </row>
@@ -17956,28 +17953,28 @@
         <v>44279</v>
       </c>
       <c r="H130" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I130" s="83">
         <v>1741</v>
       </c>
       <c r="J130" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="K130" s="11" t="s">
         <v>563</v>
       </c>
-      <c r="K130" s="11" t="s">
+      <c r="L130" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="L130" s="11" t="s">
-        <v>565</v>
       </c>
       <c r="M130" s="83">
         <v>1077</v>
       </c>
       <c r="N130" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="O130" s="11" t="s">
         <v>566</v>
-      </c>
-      <c r="O130" s="11" t="s">
-        <v>567</v>
       </c>
       <c r="P130" s="11" t="s">
         <v>276</v>
@@ -17986,13 +17983,13 @@
         <v>1462</v>
       </c>
       <c r="R130" s="63" t="s">
+        <v>567</v>
+      </c>
+      <c r="S130" s="13" t="s">
         <v>568</v>
       </c>
-      <c r="S130" s="13" t="s">
+      <c r="T130" s="13" t="s">
         <v>569</v>
-      </c>
-      <c r="T130" s="13" t="s">
-        <v>570</v>
       </c>
       <c r="U130" s="83"/>
       <c r="Y130" s="83"/>
@@ -18020,37 +18017,37 @@
         <v>44279</v>
       </c>
       <c r="H131" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I131" s="81"/>
       <c r="J131" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="K131" s="11" t="s">
         <v>563</v>
       </c>
-      <c r="K131" s="11" t="s">
+      <c r="L131" s="11" t="s">
         <v>564</v>
-      </c>
-      <c r="L131" s="11" t="s">
-        <v>565</v>
       </c>
       <c r="M131" s="81"/>
       <c r="N131" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="O131" s="11" t="s">
         <v>566</v>
-      </c>
-      <c r="O131" s="11" t="s">
-        <v>567</v>
       </c>
       <c r="P131" s="11" t="s">
         <v>276</v>
       </c>
       <c r="Q131" s="81"/>
       <c r="R131" s="63" t="s">
+        <v>567</v>
+      </c>
+      <c r="S131" s="13" t="s">
         <v>568</v>
       </c>
-      <c r="S131" s="13" t="s">
+      <c r="T131" s="13" t="s">
         <v>569</v>
-      </c>
-      <c r="T131" s="13" t="s">
-        <v>570</v>
       </c>
       <c r="U131" s="81"/>
       <c r="Y131" s="81"/>
@@ -18072,13 +18069,13 @@
         <v>44279</v>
       </c>
       <c r="F132" s="52" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G132" s="50">
         <v>44279</v>
       </c>
       <c r="H132" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I132" s="83"/>
       <c r="M132" s="83"/>
@@ -18103,13 +18100,13 @@
         <v>44279</v>
       </c>
       <c r="F133" s="52" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G133" s="50">
         <v>44279</v>
       </c>
       <c r="H133" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I133" s="81"/>
       <c r="M133" s="81"/>
@@ -18134,36 +18131,36 @@
         <v>44279</v>
       </c>
       <c r="F134" s="52" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G134" s="50">
         <v>44279</v>
       </c>
       <c r="H134" s="52" t="s">
-        <v>627</v>
-      </c>
-      <c r="I134" s="91">
+        <v>626</v>
+      </c>
+      <c r="I134" s="85">
         <v>1109</v>
       </c>
       <c r="J134" s="13" t="s">
-        <v>571</v>
-      </c>
-      <c r="M134" s="88">
+        <v>570</v>
+      </c>
+      <c r="M134" s="86">
         <v>1729</v>
       </c>
       <c r="N134" s="33" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O134" s="33"/>
       <c r="P134" s="33"/>
-      <c r="Q134" s="88">
+      <c r="Q134" s="86">
         <v>1749</v>
       </c>
-      <c r="U134" s="88">
+      <c r="U134" s="86">
         <v>1787</v>
       </c>
       <c r="V134" s="62" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="W134" s="62" t="s">
         <v>454</v>
@@ -18190,23 +18187,23 @@
         <v>44279</v>
       </c>
       <c r="F135" s="52" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G135" s="50">
         <v>44280</v>
       </c>
       <c r="H135" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I135" s="81"/>
       <c r="J135" s="62" t="s">
+        <v>572</v>
+      </c>
+      <c r="K135" s="62" t="s">
         <v>573</v>
       </c>
-      <c r="K135" s="62" t="s">
+      <c r="L135" s="68" t="s">
         <v>574</v>
-      </c>
-      <c r="L135" s="68" t="s">
-        <v>575</v>
       </c>
       <c r="M135" s="81"/>
       <c r="N135" s="33" t="s">
@@ -18221,7 +18218,7 @@
       <c r="Q135" s="81"/>
       <c r="U135" s="81"/>
       <c r="V135" s="62" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="W135" s="62" t="s">
         <v>454</v>
@@ -18248,25 +18245,25 @@
         <v>44279</v>
       </c>
       <c r="F136" s="52" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G136" s="50">
         <v>44279</v>
       </c>
       <c r="H136" s="52" t="s">
-        <v>629</v>
-      </c>
-      <c r="I136" s="88">
+        <v>628</v>
+      </c>
+      <c r="I136" s="86">
         <v>1796</v>
       </c>
-      <c r="M136" s="88">
+      <c r="M136" s="86">
         <v>1058</v>
       </c>
-      <c r="Q136" s="88">
+      <c r="Q136" s="86">
         <v>1282</v>
       </c>
       <c r="R136" s="13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="U136" s="83"/>
       <c r="Y136" s="83"/>
@@ -18288,25 +18285,25 @@
         <v>44280</v>
       </c>
       <c r="F137" s="52" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G137" s="50">
         <v>44280</v>
       </c>
       <c r="H137" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I137" s="81"/>
       <c r="M137" s="81"/>
       <c r="Q137" s="81"/>
       <c r="R137" s="69" t="s">
+        <v>575</v>
+      </c>
+      <c r="S137" s="62" t="s">
         <v>576</v>
       </c>
-      <c r="S137" s="62" t="s">
+      <c r="T137" s="67" t="s">
         <v>577</v>
-      </c>
-      <c r="T137" s="67" t="s">
-        <v>578</v>
       </c>
       <c r="U137" s="81"/>
       <c r="Y137" s="81"/>
@@ -18381,17 +18378,17 @@
       <c r="H140" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="I140" s="85" t="s">
-        <v>293</v>
+      <c r="I140" s="89">
+        <v>9992</v>
       </c>
       <c r="J140" s="49" t="s">
+        <v>578</v>
+      </c>
+      <c r="K140" s="49" t="s">
         <v>579</v>
       </c>
-      <c r="K140" s="49" t="s">
+      <c r="L140" s="49" t="s">
         <v>580</v>
-      </c>
-      <c r="L140" s="49" t="s">
-        <v>581</v>
       </c>
       <c r="M140" s="51"/>
       <c r="Q140" s="51"/>
@@ -18425,13 +18422,13 @@
       </c>
       <c r="I141" s="81"/>
       <c r="J141" s="49" t="s">
+        <v>578</v>
+      </c>
+      <c r="K141" s="49" t="s">
         <v>579</v>
       </c>
-      <c r="K141" s="49" t="s">
+      <c r="L141" s="49" t="s">
         <v>580</v>
-      </c>
-      <c r="L141" s="49" t="s">
-        <v>581</v>
       </c>
       <c r="M141" s="51"/>
       <c r="Q141" s="51"/>
@@ -18596,13 +18593,13 @@
         <v>1236</v>
       </c>
       <c r="J147" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="K147" s="13" t="s">
         <v>582</v>
       </c>
-      <c r="K147" s="13" t="s">
+      <c r="L147" s="13" t="s">
         <v>583</v>
-      </c>
-      <c r="L147" s="13" t="s">
-        <v>584</v>
       </c>
       <c r="Q147" s="83"/>
       <c r="U147" s="83"/>
@@ -18635,25 +18632,25 @@
       </c>
       <c r="I148" s="81"/>
       <c r="J148" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="K148" s="13" t="s">
         <v>582</v>
       </c>
-      <c r="K148" s="13" t="s">
+      <c r="L148" s="13" t="s">
         <v>583</v>
-      </c>
-      <c r="L148" s="13" t="s">
-        <v>584</v>
       </c>
       <c r="M148" s="71">
         <v>1481</v>
       </c>
       <c r="N148" s="72" t="s">
+        <v>584</v>
+      </c>
+      <c r="O148" s="72" t="s">
         <v>585</v>
       </c>
-      <c r="O148" s="72" t="s">
+      <c r="P148" s="73" t="s">
         <v>586</v>
-      </c>
-      <c r="P148" s="73" t="s">
-        <v>587</v>
       </c>
       <c r="Q148" s="81"/>
       <c r="U148" s="81"/>
@@ -18776,25 +18773,25 @@
         <v>1422</v>
       </c>
       <c r="R152" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="S152" s="13" t="s">
         <v>588</v>
       </c>
-      <c r="S152" s="13" t="s">
+      <c r="T152" s="13" t="s">
         <v>589</v>
-      </c>
-      <c r="T152" s="13" t="s">
-        <v>590</v>
       </c>
       <c r="U152" s="83">
         <v>1544</v>
       </c>
       <c r="V152" s="13" t="s">
+        <v>590</v>
+      </c>
+      <c r="W152" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="W152" s="13" t="s">
+      <c r="X152" s="13" t="s">
         <v>592</v>
-      </c>
-      <c r="X152" s="13" t="s">
-        <v>593</v>
       </c>
       <c r="Y152" s="83"/>
     </row>
@@ -18827,23 +18824,23 @@
       <c r="M153" s="81"/>
       <c r="Q153" s="81"/>
       <c r="R153" s="13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="S153" s="30" t="s">
+        <v>588</v>
+      </c>
+      <c r="T153" s="13" t="s">
         <v>589</v>
-      </c>
-      <c r="T153" s="13" t="s">
-        <v>590</v>
       </c>
       <c r="U153" s="81"/>
       <c r="V153" s="13" t="s">
+        <v>590</v>
+      </c>
+      <c r="W153" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="W153" s="13" t="s">
+      <c r="X153" s="13" t="s">
         <v>592</v>
-      </c>
-      <c r="X153" s="13" t="s">
-        <v>593</v>
       </c>
       <c r="Y153" s="81"/>
     </row>
@@ -18934,29 +18931,29 @@
       <c r="H156" s="52" t="s">
         <v>298</v>
       </c>
-      <c r="I156" s="88">
+      <c r="I156" s="86">
         <v>1517</v>
       </c>
       <c r="J156" s="13" t="s">
+        <v>594</v>
+      </c>
+      <c r="K156" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="K156" s="13" t="s">
+      <c r="L156" s="75" t="s">
         <v>596</v>
       </c>
-      <c r="L156" s="75" t="s">
+      <c r="M156" s="86">
+        <v>1083</v>
+      </c>
+      <c r="N156" s="13" t="s">
         <v>597</v>
       </c>
-      <c r="M156" s="88">
-        <v>1083</v>
-      </c>
-      <c r="N156" s="13" t="s">
+      <c r="O156" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="O156" s="13" t="s">
+      <c r="P156" s="76" t="s">
         <v>599</v>
-      </c>
-      <c r="P156" s="76" t="s">
-        <v>600</v>
       </c>
       <c r="Q156" s="83">
         <v>1174</v>
@@ -18991,23 +18988,23 @@
       </c>
       <c r="I157" s="81"/>
       <c r="J157" s="13" t="s">
+        <v>594</v>
+      </c>
+      <c r="K157" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="K157" s="13" t="s">
+      <c r="L157" s="75" t="s">
         <v>596</v>
-      </c>
-      <c r="L157" s="75" t="s">
-        <v>597</v>
       </c>
       <c r="M157" s="81"/>
       <c r="N157" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="O157" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="O157" s="13" t="s">
+      <c r="P157" s="76" t="s">
         <v>599</v>
-      </c>
-      <c r="P157" s="76" t="s">
-        <v>600</v>
       </c>
       <c r="Q157" s="81"/>
       <c r="U157" s="81"/>
@@ -19276,49 +19273,49 @@
         <v>1494</v>
       </c>
       <c r="J166" s="13" t="s">
+        <v>600</v>
+      </c>
+      <c r="K166" s="13" t="s">
         <v>601</v>
       </c>
-      <c r="K166" s="13" t="s">
+      <c r="L166" s="63" t="s">
         <v>602</v>
-      </c>
-      <c r="L166" s="63" t="s">
-        <v>603</v>
       </c>
       <c r="M166" s="83">
         <v>1498</v>
       </c>
       <c r="N166" s="13" t="s">
+        <v>603</v>
+      </c>
+      <c r="O166" s="13" t="s">
         <v>604</v>
       </c>
-      <c r="O166" s="13" t="s">
+      <c r="P166" s="63" t="s">
         <v>605</v>
-      </c>
-      <c r="P166" s="63" t="s">
-        <v>606</v>
       </c>
       <c r="Q166" s="83">
         <v>1516</v>
       </c>
       <c r="R166" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="S166" s="13" t="s">
         <v>607</v>
       </c>
-      <c r="S166" s="13" t="s">
+      <c r="T166" s="63" t="s">
         <v>608</v>
-      </c>
-      <c r="T166" s="63" t="s">
-        <v>609</v>
       </c>
       <c r="U166" s="83">
         <v>1602</v>
       </c>
       <c r="V166" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="W166" s="13" t="s">
         <v>610</v>
       </c>
-      <c r="W166" s="13" t="s">
+      <c r="X166" s="63" t="s">
         <v>611</v>
-      </c>
-      <c r="X166" s="63" t="s">
-        <v>612</v>
       </c>
       <c r="Y166" s="83"/>
     </row>
@@ -19349,43 +19346,43 @@
       </c>
       <c r="I167" s="81"/>
       <c r="J167" s="13" t="s">
+        <v>600</v>
+      </c>
+      <c r="K167" s="13" t="s">
         <v>601</v>
       </c>
-      <c r="K167" s="13" t="s">
+      <c r="L167" s="63" t="s">
         <v>602</v>
-      </c>
-      <c r="L167" s="63" t="s">
-        <v>603</v>
       </c>
       <c r="M167" s="81"/>
       <c r="N167" s="13" t="s">
+        <v>603</v>
+      </c>
+      <c r="O167" s="13" t="s">
         <v>604</v>
       </c>
-      <c r="O167" s="13" t="s">
+      <c r="P167" s="63" t="s">
         <v>605</v>
-      </c>
-      <c r="P167" s="63" t="s">
-        <v>606</v>
       </c>
       <c r="Q167" s="81"/>
       <c r="R167" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="S167" s="13" t="s">
         <v>607</v>
       </c>
-      <c r="S167" s="13" t="s">
+      <c r="T167" s="63" t="s">
         <v>608</v>
-      </c>
-      <c r="T167" s="63" t="s">
-        <v>609</v>
       </c>
       <c r="U167" s="81"/>
       <c r="V167" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="W167" s="13" t="s">
         <v>610</v>
       </c>
-      <c r="W167" s="13" t="s">
+      <c r="X167" s="63" t="s">
         <v>611</v>
-      </c>
-      <c r="X167" s="63" t="s">
-        <v>612</v>
       </c>
       <c r="Y167" s="81"/>
     </row>
@@ -19418,19 +19415,19 @@
         <v>1760</v>
       </c>
       <c r="J168" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="K168" s="13" t="s">
         <v>613</v>
       </c>
-      <c r="K168" s="13" t="s">
+      <c r="L168" s="63" t="s">
         <v>614</v>
       </c>
-      <c r="L168" s="63" t="s">
+      <c r="M168" s="90">
+        <v>1237</v>
+      </c>
+      <c r="N168" s="11" t="s">
         <v>615</v>
-      </c>
-      <c r="M168" s="89">
-        <v>1237</v>
-      </c>
-      <c r="N168" s="11" t="s">
-        <v>616</v>
       </c>
       <c r="O168" s="77" t="s">
         <v>411</v>
@@ -19438,29 +19435,29 @@
       <c r="P168" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="Q168" s="90">
+      <c r="Q168" s="84">
         <v>1488</v>
       </c>
       <c r="R168" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="S168" s="78" t="s">
         <v>617</v>
       </c>
-      <c r="S168" s="78" t="s">
+      <c r="T168" s="11" t="s">
         <v>618</v>
       </c>
-      <c r="T168" s="11" t="s">
+      <c r="U168" s="84">
+        <v>1765</v>
+      </c>
+      <c r="V168" s="79" t="s">
         <v>619</v>
       </c>
-      <c r="U168" s="90">
-        <v>1765</v>
-      </c>
-      <c r="V168" s="79" t="s">
+      <c r="W168" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="W168" s="11" t="s">
+      <c r="X168" s="11" t="s">
         <v>621</v>
-      </c>
-      <c r="X168" s="11" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="169" spans="1:25" ht="15.75" customHeight="1">
@@ -19490,17 +19487,17 @@
       </c>
       <c r="I169" s="81"/>
       <c r="J169" s="13" t="s">
+        <v>612</v>
+      </c>
+      <c r="K169" s="13" t="s">
         <v>613</v>
       </c>
-      <c r="K169" s="13" t="s">
+      <c r="L169" s="63" t="s">
         <v>614</v>
-      </c>
-      <c r="L169" s="63" t="s">
-        <v>615</v>
       </c>
       <c r="M169" s="81"/>
       <c r="N169" s="11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="O169" s="77" t="s">
         <v>411</v>
@@ -19510,23 +19507,23 @@
       </c>
       <c r="Q169" s="81"/>
       <c r="R169" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="S169" s="78" t="s">
         <v>617</v>
       </c>
-      <c r="S169" s="78" t="s">
+      <c r="T169" s="11" t="s">
         <v>618</v>
-      </c>
-      <c r="T169" s="11" t="s">
-        <v>619</v>
       </c>
       <c r="U169" s="81"/>
       <c r="V169" s="79" t="s">
+        <v>619</v>
+      </c>
+      <c r="W169" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="W169" s="11" t="s">
+      <c r="X169" s="11" t="s">
         <v>621</v>
-      </c>
-      <c r="X169" s="11" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="170" spans="1:25" ht="15.75" customHeight="1">
@@ -21227,98 +21224,241 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="355">
-    <mergeCell ref="U112:U113"/>
-    <mergeCell ref="U114:U115"/>
-    <mergeCell ref="U116:U117"/>
-    <mergeCell ref="U118:U119"/>
-    <mergeCell ref="U121:U122"/>
-    <mergeCell ref="U123:U124"/>
-    <mergeCell ref="U125:U126"/>
-    <mergeCell ref="U127:U128"/>
-    <mergeCell ref="U130:U131"/>
-    <mergeCell ref="U88:U89"/>
-    <mergeCell ref="U94:U95"/>
-    <mergeCell ref="U96:U97"/>
-    <mergeCell ref="U98:U99"/>
-    <mergeCell ref="U100:U101"/>
-    <mergeCell ref="U103:U104"/>
-    <mergeCell ref="U105:U106"/>
-    <mergeCell ref="U107:U108"/>
-    <mergeCell ref="U109:U110"/>
-    <mergeCell ref="U68:U69"/>
-    <mergeCell ref="U70:U71"/>
-    <mergeCell ref="U73:U74"/>
-    <mergeCell ref="U75:U76"/>
-    <mergeCell ref="U77:U78"/>
-    <mergeCell ref="U79:U80"/>
-    <mergeCell ref="U82:U83"/>
-    <mergeCell ref="U84:U85"/>
-    <mergeCell ref="U86:U87"/>
-    <mergeCell ref="U46:U47"/>
-    <mergeCell ref="U48:U49"/>
-    <mergeCell ref="U50:U51"/>
-    <mergeCell ref="U52:U53"/>
-    <mergeCell ref="U57:U58"/>
-    <mergeCell ref="U59:U60"/>
-    <mergeCell ref="U61:U62"/>
-    <mergeCell ref="U64:U65"/>
-    <mergeCell ref="U66:U67"/>
-    <mergeCell ref="U168:U169"/>
-    <mergeCell ref="U170:U171"/>
-    <mergeCell ref="Y170:Y171"/>
-    <mergeCell ref="Y173:Y174"/>
-    <mergeCell ref="Y175:Y176"/>
-    <mergeCell ref="Y177:Y178"/>
-    <mergeCell ref="U173:U174"/>
-    <mergeCell ref="U175:U176"/>
-    <mergeCell ref="U177:U178"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="I127:I128"/>
-    <mergeCell ref="I130:I131"/>
-    <mergeCell ref="I132:I133"/>
-    <mergeCell ref="I134:I135"/>
-    <mergeCell ref="U163:U164"/>
-    <mergeCell ref="U166:U167"/>
-    <mergeCell ref="Y166:Y167"/>
-    <mergeCell ref="U147:U148"/>
-    <mergeCell ref="U149:U150"/>
-    <mergeCell ref="U152:U153"/>
-    <mergeCell ref="U154:U155"/>
-    <mergeCell ref="U156:U157"/>
-    <mergeCell ref="U159:U160"/>
-    <mergeCell ref="U161:U162"/>
-    <mergeCell ref="U132:U133"/>
-    <mergeCell ref="U134:U135"/>
-    <mergeCell ref="U136:U137"/>
-    <mergeCell ref="U145:U146"/>
-    <mergeCell ref="I103:I104"/>
-    <mergeCell ref="I105:I106"/>
-    <mergeCell ref="I107:I108"/>
-    <mergeCell ref="I109:I110"/>
-    <mergeCell ref="I112:I113"/>
-    <mergeCell ref="I114:I115"/>
-    <mergeCell ref="I116:I117"/>
-    <mergeCell ref="I118:I119"/>
-    <mergeCell ref="I121:I122"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="I84:I85"/>
-    <mergeCell ref="I86:I87"/>
-    <mergeCell ref="I88:I89"/>
-    <mergeCell ref="I94:I95"/>
-    <mergeCell ref="I96:I97"/>
-    <mergeCell ref="I98:I99"/>
-    <mergeCell ref="I100:I101"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="I61:I62"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="Y161:Y162"/>
+    <mergeCell ref="Y163:Y164"/>
+    <mergeCell ref="Y145:Y146"/>
+    <mergeCell ref="Y147:Y148"/>
+    <mergeCell ref="Y149:Y150"/>
+    <mergeCell ref="Y152:Y153"/>
+    <mergeCell ref="Y154:Y155"/>
+    <mergeCell ref="Y156:Y157"/>
+    <mergeCell ref="Y159:Y160"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="Y14:Y15"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="Y18:Y19"/>
+    <mergeCell ref="Y21:Y22"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Y25:Y26"/>
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="Y48:Y49"/>
+    <mergeCell ref="Y50:Y51"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="Y55:Y56"/>
+    <mergeCell ref="Y57:Y58"/>
+    <mergeCell ref="Y59:Y60"/>
+    <mergeCell ref="Y61:Y62"/>
+    <mergeCell ref="Y64:Y65"/>
+    <mergeCell ref="Y66:Y67"/>
+    <mergeCell ref="Y68:Y69"/>
+    <mergeCell ref="Y70:Y71"/>
+    <mergeCell ref="Y73:Y74"/>
+    <mergeCell ref="Y75:Y76"/>
+    <mergeCell ref="Y77:Y78"/>
+    <mergeCell ref="Y79:Y80"/>
+    <mergeCell ref="Y82:Y83"/>
+    <mergeCell ref="Y84:Y85"/>
+    <mergeCell ref="Y86:Y87"/>
+    <mergeCell ref="Y88:Y89"/>
+    <mergeCell ref="Y94:Y95"/>
+    <mergeCell ref="Y96:Y97"/>
+    <mergeCell ref="Y98:Y99"/>
+    <mergeCell ref="Y100:Y101"/>
+    <mergeCell ref="Y103:Y104"/>
+    <mergeCell ref="Y105:Y106"/>
+    <mergeCell ref="Y107:Y108"/>
+    <mergeCell ref="Y109:Y110"/>
+    <mergeCell ref="Y112:Y113"/>
+    <mergeCell ref="Y114:Y115"/>
+    <mergeCell ref="Y116:Y117"/>
+    <mergeCell ref="Y118:Y119"/>
+    <mergeCell ref="Y121:Y122"/>
+    <mergeCell ref="Y123:Y124"/>
+    <mergeCell ref="Y125:Y126"/>
+    <mergeCell ref="Y127:Y128"/>
+    <mergeCell ref="Y130:Y131"/>
+    <mergeCell ref="Y132:Y133"/>
+    <mergeCell ref="Y134:Y135"/>
+    <mergeCell ref="Y136:Y137"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="Y30:Y31"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="Y32:Y33"/>
+    <mergeCell ref="U35:U36"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="Y35:Y36"/>
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="Q37:Q38"/>
+    <mergeCell ref="U37:U38"/>
+    <mergeCell ref="Y37:Y38"/>
+    <mergeCell ref="U39:U40"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="Q39:Q40"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="U21:U22"/>
+    <mergeCell ref="U23:U24"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="M68:M69"/>
+    <mergeCell ref="M70:M71"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="M79:M80"/>
+    <mergeCell ref="M82:M83"/>
+    <mergeCell ref="M84:M85"/>
+    <mergeCell ref="M86:M87"/>
+    <mergeCell ref="M88:M89"/>
+    <mergeCell ref="M94:M95"/>
+    <mergeCell ref="M96:M97"/>
+    <mergeCell ref="M98:M99"/>
+    <mergeCell ref="M100:M101"/>
+    <mergeCell ref="M107:M108"/>
+    <mergeCell ref="M109:M110"/>
+    <mergeCell ref="M112:M113"/>
+    <mergeCell ref="M114:M115"/>
+    <mergeCell ref="M116:M117"/>
+    <mergeCell ref="M118:M119"/>
+    <mergeCell ref="M121:M122"/>
+    <mergeCell ref="M123:M124"/>
+    <mergeCell ref="M125:M126"/>
+    <mergeCell ref="M127:M128"/>
+    <mergeCell ref="M130:M131"/>
+    <mergeCell ref="M132:M133"/>
+    <mergeCell ref="M134:M135"/>
+    <mergeCell ref="M136:M137"/>
+    <mergeCell ref="M163:M164"/>
+    <mergeCell ref="M166:M167"/>
+    <mergeCell ref="M168:M169"/>
+    <mergeCell ref="M170:M171"/>
+    <mergeCell ref="M173:M174"/>
+    <mergeCell ref="M175:M176"/>
+    <mergeCell ref="M177:M178"/>
+    <mergeCell ref="M145:M146"/>
+    <mergeCell ref="M149:M150"/>
+    <mergeCell ref="M152:M153"/>
+    <mergeCell ref="M154:M155"/>
+    <mergeCell ref="M156:M157"/>
+    <mergeCell ref="M159:M160"/>
+    <mergeCell ref="M161:M162"/>
+    <mergeCell ref="Q103:Q104"/>
+    <mergeCell ref="Q105:Q106"/>
+    <mergeCell ref="Q107:Q108"/>
+    <mergeCell ref="Q109:Q110"/>
+    <mergeCell ref="Q112:Q113"/>
+    <mergeCell ref="Q114:Q115"/>
+    <mergeCell ref="Q116:Q117"/>
+    <mergeCell ref="Q118:Q119"/>
+    <mergeCell ref="Q121:Q122"/>
+    <mergeCell ref="Q123:Q124"/>
+    <mergeCell ref="Q125:Q126"/>
+    <mergeCell ref="Q127:Q128"/>
+    <mergeCell ref="Q130:Q131"/>
+    <mergeCell ref="Q132:Q133"/>
+    <mergeCell ref="Q134:Q135"/>
+    <mergeCell ref="Q136:Q137"/>
+    <mergeCell ref="Q145:Q146"/>
+    <mergeCell ref="Q147:Q148"/>
+    <mergeCell ref="Q173:Q174"/>
+    <mergeCell ref="Q175:Q176"/>
+    <mergeCell ref="Q177:Q178"/>
+    <mergeCell ref="Q156:Q157"/>
+    <mergeCell ref="Q159:Q160"/>
+    <mergeCell ref="Q161:Q162"/>
+    <mergeCell ref="Q163:Q164"/>
+    <mergeCell ref="Q166:Q167"/>
+    <mergeCell ref="Q168:Q169"/>
+    <mergeCell ref="Q170:Q171"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="Q46:Q47"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="Q48:Q49"/>
+    <mergeCell ref="Q50:Q51"/>
+    <mergeCell ref="M50:M51"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="M55:M56"/>
+    <mergeCell ref="M57:M58"/>
+    <mergeCell ref="M59:M60"/>
+    <mergeCell ref="M64:M65"/>
+    <mergeCell ref="M66:M67"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="Q55:Q56"/>
+    <mergeCell ref="Q57:Q58"/>
+    <mergeCell ref="Q59:Q60"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="Q64:Q65"/>
+    <mergeCell ref="Q66:Q67"/>
+    <mergeCell ref="I149:I150"/>
+    <mergeCell ref="I152:I153"/>
+    <mergeCell ref="I154:I155"/>
+    <mergeCell ref="I173:I174"/>
+    <mergeCell ref="I175:I176"/>
+    <mergeCell ref="Q68:Q69"/>
+    <mergeCell ref="Q70:Q71"/>
+    <mergeCell ref="Q73:Q74"/>
+    <mergeCell ref="Q75:Q76"/>
+    <mergeCell ref="Q77:Q78"/>
+    <mergeCell ref="Q79:Q80"/>
+    <mergeCell ref="Q82:Q83"/>
+    <mergeCell ref="M103:M104"/>
+    <mergeCell ref="M105:M106"/>
+    <mergeCell ref="Q84:Q85"/>
+    <mergeCell ref="Q86:Q87"/>
+    <mergeCell ref="Q88:Q89"/>
+    <mergeCell ref="Q94:Q95"/>
+    <mergeCell ref="Q96:Q97"/>
+    <mergeCell ref="Q98:Q99"/>
+    <mergeCell ref="Q100:Q101"/>
+    <mergeCell ref="Q149:Q150"/>
+    <mergeCell ref="Q152:Q153"/>
+    <mergeCell ref="Q154:Q155"/>
     <mergeCell ref="I177:I178"/>
     <mergeCell ref="I156:I157"/>
     <mergeCell ref="I159:I160"/>
@@ -21343,245 +21483,102 @@
     <mergeCell ref="I52:I53"/>
     <mergeCell ref="I55:I56"/>
     <mergeCell ref="I57:I58"/>
+    <mergeCell ref="I59:I60"/>
+    <mergeCell ref="I61:I62"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="I75:I76"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="I94:I95"/>
+    <mergeCell ref="I96:I97"/>
+    <mergeCell ref="I98:I99"/>
+    <mergeCell ref="I100:I101"/>
+    <mergeCell ref="I103:I104"/>
+    <mergeCell ref="I105:I106"/>
+    <mergeCell ref="I107:I108"/>
+    <mergeCell ref="I109:I110"/>
+    <mergeCell ref="I112:I113"/>
+    <mergeCell ref="I114:I115"/>
+    <mergeCell ref="I116:I117"/>
+    <mergeCell ref="I118:I119"/>
+    <mergeCell ref="I121:I122"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="I127:I128"/>
+    <mergeCell ref="I130:I131"/>
+    <mergeCell ref="I132:I133"/>
+    <mergeCell ref="I134:I135"/>
+    <mergeCell ref="U163:U164"/>
+    <mergeCell ref="U166:U167"/>
+    <mergeCell ref="Y166:Y167"/>
+    <mergeCell ref="U147:U148"/>
+    <mergeCell ref="U149:U150"/>
+    <mergeCell ref="U152:U153"/>
+    <mergeCell ref="U154:U155"/>
+    <mergeCell ref="U156:U157"/>
+    <mergeCell ref="U159:U160"/>
+    <mergeCell ref="U161:U162"/>
+    <mergeCell ref="U132:U133"/>
+    <mergeCell ref="U134:U135"/>
+    <mergeCell ref="U136:U137"/>
+    <mergeCell ref="U145:U146"/>
     <mergeCell ref="I136:I137"/>
     <mergeCell ref="I140:I141"/>
     <mergeCell ref="I145:I146"/>
     <mergeCell ref="I147:I148"/>
-    <mergeCell ref="I149:I150"/>
-    <mergeCell ref="I152:I153"/>
-    <mergeCell ref="I154:I155"/>
-    <mergeCell ref="I173:I174"/>
-    <mergeCell ref="I175:I176"/>
-    <mergeCell ref="Q68:Q69"/>
-    <mergeCell ref="Q70:Q71"/>
-    <mergeCell ref="Q73:Q74"/>
-    <mergeCell ref="Q75:Q76"/>
-    <mergeCell ref="Q77:Q78"/>
-    <mergeCell ref="Q79:Q80"/>
-    <mergeCell ref="Q82:Q83"/>
-    <mergeCell ref="M103:M104"/>
-    <mergeCell ref="M105:M106"/>
-    <mergeCell ref="Q84:Q85"/>
-    <mergeCell ref="Q86:Q87"/>
-    <mergeCell ref="Q88:Q89"/>
-    <mergeCell ref="Q94:Q95"/>
-    <mergeCell ref="Q96:Q97"/>
-    <mergeCell ref="Q98:Q99"/>
-    <mergeCell ref="Q100:Q101"/>
-    <mergeCell ref="M59:M60"/>
-    <mergeCell ref="M64:M65"/>
-    <mergeCell ref="M66:M67"/>
-    <mergeCell ref="Q52:Q53"/>
-    <mergeCell ref="Q55:Q56"/>
-    <mergeCell ref="Q57:Q58"/>
-    <mergeCell ref="Q59:Q60"/>
-    <mergeCell ref="Q61:Q62"/>
-    <mergeCell ref="Q64:Q65"/>
-    <mergeCell ref="Q66:Q67"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="Q46:Q47"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="Q48:Q49"/>
-    <mergeCell ref="Q50:Q51"/>
-    <mergeCell ref="M50:M51"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="M55:M56"/>
-    <mergeCell ref="M57:M58"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="Q149:Q150"/>
-    <mergeCell ref="Q152:Q153"/>
-    <mergeCell ref="Q154:Q155"/>
-    <mergeCell ref="Q173:Q174"/>
-    <mergeCell ref="Q175:Q176"/>
-    <mergeCell ref="Q177:Q178"/>
-    <mergeCell ref="Q156:Q157"/>
-    <mergeCell ref="Q159:Q160"/>
-    <mergeCell ref="Q161:Q162"/>
-    <mergeCell ref="Q163:Q164"/>
-    <mergeCell ref="Q166:Q167"/>
-    <mergeCell ref="Q168:Q169"/>
-    <mergeCell ref="Q170:Q171"/>
-    <mergeCell ref="Q123:Q124"/>
-    <mergeCell ref="Q125:Q126"/>
-    <mergeCell ref="Q127:Q128"/>
-    <mergeCell ref="Q130:Q131"/>
-    <mergeCell ref="Q132:Q133"/>
-    <mergeCell ref="Q134:Q135"/>
-    <mergeCell ref="Q136:Q137"/>
-    <mergeCell ref="Q145:Q146"/>
-    <mergeCell ref="Q147:Q148"/>
-    <mergeCell ref="Q103:Q104"/>
-    <mergeCell ref="Q105:Q106"/>
-    <mergeCell ref="Q107:Q108"/>
-    <mergeCell ref="Q109:Q110"/>
-    <mergeCell ref="Q112:Q113"/>
-    <mergeCell ref="Q114:Q115"/>
-    <mergeCell ref="Q116:Q117"/>
-    <mergeCell ref="Q118:Q119"/>
-    <mergeCell ref="Q121:Q122"/>
-    <mergeCell ref="M136:M137"/>
-    <mergeCell ref="M163:M164"/>
-    <mergeCell ref="M166:M167"/>
-    <mergeCell ref="M168:M169"/>
-    <mergeCell ref="M170:M171"/>
-    <mergeCell ref="M173:M174"/>
-    <mergeCell ref="M175:M176"/>
-    <mergeCell ref="M177:M178"/>
-    <mergeCell ref="M145:M146"/>
-    <mergeCell ref="M149:M150"/>
-    <mergeCell ref="M152:M153"/>
-    <mergeCell ref="M154:M155"/>
-    <mergeCell ref="M156:M157"/>
-    <mergeCell ref="M159:M160"/>
-    <mergeCell ref="M161:M162"/>
-    <mergeCell ref="M116:M117"/>
-    <mergeCell ref="M118:M119"/>
-    <mergeCell ref="M121:M122"/>
-    <mergeCell ref="M123:M124"/>
-    <mergeCell ref="M125:M126"/>
-    <mergeCell ref="M127:M128"/>
-    <mergeCell ref="M130:M131"/>
-    <mergeCell ref="M132:M133"/>
-    <mergeCell ref="M134:M135"/>
-    <mergeCell ref="M88:M89"/>
-    <mergeCell ref="M94:M95"/>
-    <mergeCell ref="M96:M97"/>
-    <mergeCell ref="M98:M99"/>
-    <mergeCell ref="M100:M101"/>
-    <mergeCell ref="M107:M108"/>
-    <mergeCell ref="M109:M110"/>
-    <mergeCell ref="M112:M113"/>
-    <mergeCell ref="M114:M115"/>
-    <mergeCell ref="M68:M69"/>
-    <mergeCell ref="M70:M71"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="M77:M78"/>
-    <mergeCell ref="M79:M80"/>
-    <mergeCell ref="M82:M83"/>
-    <mergeCell ref="M84:M85"/>
-    <mergeCell ref="M86:M87"/>
-    <mergeCell ref="Y35:Y36"/>
-    <mergeCell ref="Q35:Q36"/>
-    <mergeCell ref="Q37:Q38"/>
-    <mergeCell ref="U37:U38"/>
-    <mergeCell ref="Y37:Y38"/>
-    <mergeCell ref="U39:U40"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="Q39:Q40"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="U21:U22"/>
-    <mergeCell ref="U23:U24"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="Y130:Y131"/>
-    <mergeCell ref="Y132:Y133"/>
-    <mergeCell ref="Y134:Y135"/>
-    <mergeCell ref="Y136:Y137"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="Y30:Y31"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="Q32:Q33"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="Y32:Y33"/>
-    <mergeCell ref="U35:U36"/>
-    <mergeCell ref="Y109:Y110"/>
-    <mergeCell ref="Y112:Y113"/>
-    <mergeCell ref="Y114:Y115"/>
-    <mergeCell ref="Y116:Y117"/>
-    <mergeCell ref="Y118:Y119"/>
-    <mergeCell ref="Y121:Y122"/>
-    <mergeCell ref="Y123:Y124"/>
-    <mergeCell ref="Y125:Y126"/>
-    <mergeCell ref="Y127:Y128"/>
-    <mergeCell ref="Y86:Y87"/>
-    <mergeCell ref="Y88:Y89"/>
-    <mergeCell ref="Y94:Y95"/>
-    <mergeCell ref="Y96:Y97"/>
-    <mergeCell ref="Y98:Y99"/>
-    <mergeCell ref="Y100:Y101"/>
-    <mergeCell ref="Y103:Y104"/>
-    <mergeCell ref="Y105:Y106"/>
-    <mergeCell ref="Y107:Y108"/>
-    <mergeCell ref="Y66:Y67"/>
-    <mergeCell ref="Y68:Y69"/>
-    <mergeCell ref="Y70:Y71"/>
-    <mergeCell ref="Y73:Y74"/>
-    <mergeCell ref="Y75:Y76"/>
-    <mergeCell ref="Y77:Y78"/>
-    <mergeCell ref="Y79:Y80"/>
-    <mergeCell ref="Y82:Y83"/>
-    <mergeCell ref="Y84:Y85"/>
-    <mergeCell ref="Y46:Y47"/>
-    <mergeCell ref="Y48:Y49"/>
-    <mergeCell ref="Y50:Y51"/>
-    <mergeCell ref="Y52:Y53"/>
-    <mergeCell ref="Y55:Y56"/>
-    <mergeCell ref="Y57:Y58"/>
-    <mergeCell ref="Y59:Y60"/>
-    <mergeCell ref="Y61:Y62"/>
-    <mergeCell ref="Y64:Y65"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="Y14:Y15"/>
-    <mergeCell ref="Y16:Y17"/>
-    <mergeCell ref="Y18:Y19"/>
-    <mergeCell ref="Y21:Y22"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="Y25:Y26"/>
-    <mergeCell ref="Y161:Y162"/>
-    <mergeCell ref="Y163:Y164"/>
-    <mergeCell ref="Y145:Y146"/>
-    <mergeCell ref="Y147:Y148"/>
-    <mergeCell ref="Y149:Y150"/>
-    <mergeCell ref="Y152:Y153"/>
-    <mergeCell ref="Y154:Y155"/>
-    <mergeCell ref="Y156:Y157"/>
-    <mergeCell ref="Y159:Y160"/>
+    <mergeCell ref="U168:U169"/>
+    <mergeCell ref="U170:U171"/>
+    <mergeCell ref="Y170:Y171"/>
+    <mergeCell ref="Y173:Y174"/>
+    <mergeCell ref="Y175:Y176"/>
+    <mergeCell ref="Y177:Y178"/>
+    <mergeCell ref="U173:U174"/>
+    <mergeCell ref="U175:U176"/>
+    <mergeCell ref="U177:U178"/>
+    <mergeCell ref="U46:U47"/>
+    <mergeCell ref="U48:U49"/>
+    <mergeCell ref="U50:U51"/>
+    <mergeCell ref="U52:U53"/>
+    <mergeCell ref="U57:U58"/>
+    <mergeCell ref="U59:U60"/>
+    <mergeCell ref="U61:U62"/>
+    <mergeCell ref="U64:U65"/>
+    <mergeCell ref="U66:U67"/>
+    <mergeCell ref="U68:U69"/>
+    <mergeCell ref="U70:U71"/>
+    <mergeCell ref="U73:U74"/>
+    <mergeCell ref="U75:U76"/>
+    <mergeCell ref="U77:U78"/>
+    <mergeCell ref="U79:U80"/>
+    <mergeCell ref="U82:U83"/>
+    <mergeCell ref="U84:U85"/>
+    <mergeCell ref="U86:U87"/>
+    <mergeCell ref="U88:U89"/>
+    <mergeCell ref="U94:U95"/>
+    <mergeCell ref="U96:U97"/>
+    <mergeCell ref="U98:U99"/>
+    <mergeCell ref="U100:U101"/>
+    <mergeCell ref="U103:U104"/>
+    <mergeCell ref="U105:U106"/>
+    <mergeCell ref="U107:U108"/>
+    <mergeCell ref="U109:U110"/>
+    <mergeCell ref="U112:U113"/>
+    <mergeCell ref="U114:U115"/>
+    <mergeCell ref="U116:U117"/>
+    <mergeCell ref="U118:U119"/>
+    <mergeCell ref="U121:U122"/>
+    <mergeCell ref="U123:U124"/>
+    <mergeCell ref="U125:U126"/>
+    <mergeCell ref="U127:U128"/>
+    <mergeCell ref="U130:U131"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L21" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>

<commit_message>
Fix yet more import bugs, which were created by me in the first place
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/2021_sessions.xlsx
+++ b/app-server/src/main/resources/2021_sessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB747C32-07E0-EB49-97F9-478591E2DCB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1DA1EB-F5E2-7540-8C39-141942B3EEF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4082,10 +4082,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B141" sqref="B141"/>
+      <selection pane="bottomRight" activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -8770,7 +8770,7 @@
         <v>44280</v>
       </c>
       <c r="H99" s="20" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>242</v>
@@ -10222,7 +10222,7 @@
         <v>44280</v>
       </c>
       <c r="H126" s="20" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>287</v>
@@ -10712,7 +10712,7 @@
         <v>44280</v>
       </c>
       <c r="H135" s="20" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>335</v>
@@ -20170,10 +20170,10 @@
   <dimension ref="A1:AC1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="M152" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I140" sqref="I140"/>
+      <selection pane="bottomRight" activeCell="P188" sqref="P188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -26374,7 +26374,7 @@
         <v>44280</v>
       </c>
       <c r="I99" s="50" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="J99" s="95"/>
       <c r="K99" s="100" t="s">
@@ -28222,7 +28222,7 @@
         <v>44280</v>
       </c>
       <c r="I126" s="50" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="J126" s="95"/>
       <c r="K126" s="100" t="s">
@@ -28830,7 +28830,7 @@
         <v>44280</v>
       </c>
       <c r="I135" s="50" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="J135" s="95"/>
       <c r="K135" s="100" t="s">

</xml_diff>